<commit_message>
Pivot debug completed, released for live test.
</commit_message>
<xml_diff>
--- a/RT2020/Resources/Reports/Inventory/Journal/Monthly.xlsx
+++ b/RT2020/Resources/Reports/Inventory/Journal/Monthly.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\RT2020\RT2020\Resources\Reports\Inventory\Journal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B0EB73-EF12-429B-8333-86D94AC6ED03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE458E22-ADA6-4168-A253-90F5F2231422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5370" yWindow="5370" windowWidth="22260" windowHeight="14205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2430" yWindow="2580" windowWidth="27495" windowHeight="15810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>

</xml_diff>